<commit_message>
included different datasets on populism
</commit_message>
<xml_diff>
--- a/data/popuList.xlsx
+++ b/data/popuList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\ucloud\01 Studium\01 MA@UvA\00 Working\Popu-list\00 PopuList 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unihamburgde-my.sharepoint.com/personal/jasmin_sarah_koenig_uni-hamburg_de/Documents/Desktop/Dissertation/Leviathan/konstregression/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6101969B-1989-43A7-9D6B-C3411DAE7E1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{6101969B-1989-43A7-9D6B-C3411DAE7E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21EBDF9-6B82-4DCF-934E-978F4FD9CCA4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Populist 2.0 after R cleaning" sheetId="1" r:id="rId1"/>
@@ -2019,7 +2019,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2153,6 +2153,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Museo_300"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2502,7 +2507,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2510,6 +2515,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2867,16 +2873,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" topLeftCell="R12" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2971,7 +2977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31">
       <c r="A2" s="1" t="s">
         <v>576</v>
       </c>
@@ -3066,7 +3072,7 @@
         <v>42710</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31">
       <c r="A3" s="1" t="s">
         <v>577</v>
       </c>
@@ -3161,7 +3167,7 @@
         <v>42420</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -3254,7 +3260,7 @@
       </c>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -3349,7 +3355,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -3442,7 +3448,7 @@
       </c>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -3537,7 +3543,7 @@
         <v>21430</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -3630,7 +3636,7 @@
       </c>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31">
       <c r="A9" s="1" t="s">
         <v>578</v>
       </c>
@@ -3723,7 +3729,7 @@
       </c>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -3818,7 +3824,7 @@
         <v>21914</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -3913,7 +3919,7 @@
         <v>80710</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
@@ -4008,7 +4014,7 @@
         <v>80630</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -4103,7 +4109,7 @@
         <v>80901</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -4198,7 +4204,7 @@
         <v>80510</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -4291,7 +4297,7 @@
       </c>
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -4386,7 +4392,7 @@
         <v>80902</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -4481,7 +4487,7 @@
         <v>80620</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31">
       <c r="A18" s="1" t="s">
         <v>579</v>
       </c>
@@ -4574,7 +4580,7 @@
       </c>
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
@@ -4669,7 +4675,7 @@
         <v>80640</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31">
       <c r="A20" s="1" t="s">
         <v>79</v>
       </c>
@@ -4754,13 +4760,15 @@
       <c r="AB20" s="1">
         <v>0</v>
       </c>
-      <c r="AC20" s="1"/>
+      <c r="AC20" s="3">
+        <v>6620</v>
+      </c>
       <c r="AD20" s="1">
         <v>2193</v>
       </c>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -4855,7 +4863,7 @@
         <v>81713</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31">
       <c r="A22" s="1" t="s">
         <v>86</v>
       </c>
@@ -4940,13 +4948,15 @@
       <c r="AB22" s="1">
         <v>0</v>
       </c>
-      <c r="AC22" s="1"/>
+      <c r="AC22" s="3">
+        <v>3706</v>
+      </c>
       <c r="AD22" s="1">
         <v>2181</v>
       </c>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -5041,7 +5051,7 @@
         <v>81952</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31">
       <c r="A24" s="1" t="s">
         <v>580</v>
       </c>
@@ -5134,7 +5144,7 @@
       </c>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31">
       <c r="A25" s="1" t="s">
         <v>94</v>
       </c>
@@ -5227,7 +5237,7 @@
       </c>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31">
       <c r="A26" s="1" t="s">
         <v>97</v>
       </c>
@@ -5322,7 +5332,7 @@
         <v>81460</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31">
       <c r="A27" s="1" t="s">
         <v>581</v>
       </c>
@@ -5417,7 +5427,7 @@
         <v>81960</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31">
       <c r="A28" s="1" t="s">
         <v>582</v>
       </c>
@@ -5512,7 +5522,7 @@
         <v>55321</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31">
       <c r="A29" s="1" t="s">
         <v>105</v>
       </c>
@@ -5607,7 +5617,7 @@
         <v>55720</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31">
       <c r="A30" s="1" t="s">
         <v>108</v>
       </c>
@@ -5702,7 +5712,7 @@
         <v>55340</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31">
       <c r="A31" s="1" t="s">
         <v>583</v>
       </c>
@@ -5797,7 +5807,7 @@
         <v>82430</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31">
       <c r="A32" s="1" t="s">
         <v>584</v>
       </c>
@@ -5892,7 +5902,7 @@
         <v>82220</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:31">
       <c r="A33" s="1" t="s">
         <v>585</v>
       </c>
@@ -5985,7 +5995,7 @@
       </c>
       <c r="AE33" s="1"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:31">
       <c r="A34" s="1" t="s">
         <v>586</v>
       </c>
@@ -6080,7 +6090,7 @@
         <v>82710</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:31">
       <c r="A35" s="1" t="s">
         <v>587</v>
       </c>
@@ -6173,7 +6183,7 @@
       </c>
       <c r="AE35" s="1"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:31">
       <c r="A36" s="1" t="s">
         <v>588</v>
       </c>
@@ -6266,7 +6276,7 @@
       </c>
       <c r="AE36" s="1"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:31">
       <c r="A37" s="1" t="s">
         <v>589</v>
       </c>
@@ -6361,7 +6371,7 @@
         <v>82721</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:31">
       <c r="A38" s="1" t="s">
         <v>590</v>
       </c>
@@ -6456,7 +6466,7 @@
         <v>82720</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:31">
       <c r="A39" s="1" t="s">
         <v>591</v>
       </c>
@@ -6551,7 +6561,7 @@
         <v>82952</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:31">
       <c r="A40" s="1" t="s">
         <v>130</v>
       </c>
@@ -6646,7 +6656,7 @@
         <v>13720</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:31">
       <c r="A41" s="1" t="s">
         <v>592</v>
       </c>
@@ -6741,7 +6751,7 @@
         <v>13229</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:31">
       <c r="A42" s="1" t="s">
         <v>136</v>
       </c>
@@ -6836,7 +6846,7 @@
         <v>13951</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:31">
       <c r="A43" s="1" t="s">
         <v>139</v>
       </c>
@@ -6929,7 +6939,7 @@
       </c>
       <c r="AE43" s="1"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:31">
       <c r="A44" s="1" t="s">
         <v>142</v>
       </c>
@@ -7024,7 +7034,7 @@
         <v>13230</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:31">
       <c r="A45" s="1" t="s">
         <v>593</v>
       </c>
@@ -7115,7 +7125,7 @@
       </c>
       <c r="AE45" s="1"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:31">
       <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
@@ -7210,7 +7220,7 @@
         <v>83712</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:31">
       <c r="A47" s="1" t="s">
         <v>151</v>
       </c>
@@ -7305,7 +7315,7 @@
         <v>83612</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:31">
       <c r="A48" s="1" t="s">
         <v>154</v>
       </c>
@@ -7398,7 +7408,7 @@
       </c>
       <c r="AE48" s="1"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:31">
       <c r="A49" s="1" t="s">
         <v>594</v>
       </c>
@@ -7493,7 +7503,7 @@
         <v>83901</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:31">
       <c r="A50" s="1" t="s">
         <v>159</v>
       </c>
@@ -7588,7 +7598,7 @@
         <v>14221</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:31">
       <c r="A51" s="1" t="s">
         <v>163</v>
       </c>
@@ -7681,7 +7691,7 @@
       </c>
       <c r="AE51" s="1"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:31">
       <c r="A52" s="1" t="s">
         <v>166</v>
       </c>
@@ -7776,7 +7786,7 @@
         <v>14820</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:31">
       <c r="A53" s="1" t="s">
         <v>595</v>
       </c>
@@ -7869,7 +7879,7 @@
       </c>
       <c r="AE53" s="1"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31">
       <c r="A54" s="1" t="s">
         <v>172</v>
       </c>
@@ -7964,7 +7974,7 @@
         <v>31720</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:31">
       <c r="A55" s="1" t="s">
         <v>175</v>
       </c>
@@ -8059,7 +8069,7 @@
         <v>31240</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:31">
       <c r="A56" s="1" t="s">
         <v>178</v>
       </c>
@@ -8152,7 +8162,7 @@
       </c>
       <c r="AE56" s="1"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:31">
       <c r="A57" s="1" t="s">
         <v>596</v>
       </c>
@@ -8247,7 +8257,7 @@
         <v>31220</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:31">
       <c r="A58" s="1" t="s">
         <v>183</v>
       </c>
@@ -8338,7 +8348,7 @@
       </c>
       <c r="AE58" s="1"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:31">
       <c r="A59" s="1" t="s">
         <v>597</v>
       </c>
@@ -8433,7 +8443,7 @@
         <v>41953</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:31">
       <c r="A60" s="1" t="s">
         <v>189</v>
       </c>
@@ -8528,7 +8538,7 @@
         <v>41221</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:31">
       <c r="A61" s="1" t="s">
         <v>192</v>
       </c>
@@ -8623,7 +8633,7 @@
         <v>34730</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:31">
       <c r="A62" s="1" t="s">
         <v>196</v>
       </c>
@@ -8718,7 +8728,7 @@
         <v>34314</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:31">
       <c r="A63" s="1" t="s">
         <v>199</v>
       </c>
@@ -8811,7 +8821,7 @@
       </c>
       <c r="AE63" s="1"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:31">
       <c r="A64" s="1" t="s">
         <v>202</v>
       </c>
@@ -8904,7 +8914,7 @@
       </c>
       <c r="AE64" s="1"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:31">
       <c r="A65" s="1" t="s">
         <v>598</v>
       </c>
@@ -8999,7 +9009,7 @@
         <v>34210</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:31">
       <c r="A66" s="1" t="s">
         <v>599</v>
       </c>
@@ -9094,7 +9104,7 @@
         <v>34710</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:31">
       <c r="A67" s="1" t="s">
         <v>600</v>
       </c>
@@ -9189,7 +9199,7 @@
         <v>34720</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:31">
       <c r="A68" s="1" t="s">
         <v>601</v>
       </c>
@@ -9280,7 +9290,7 @@
       </c>
       <c r="AE68" s="1"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:31">
       <c r="A69" s="1" t="s">
         <v>211</v>
       </c>
@@ -9375,7 +9385,7 @@
         <v>34512</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:31">
       <c r="A70" s="1" t="s">
         <v>602</v>
       </c>
@@ -9470,7 +9480,7 @@
         <v>34020</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:31">
       <c r="A71" s="1" t="s">
         <v>603</v>
       </c>
@@ -9565,7 +9575,7 @@
         <v>34211</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:31">
       <c r="A72" s="1" t="s">
         <v>604</v>
       </c>
@@ -9658,7 +9668,7 @@
         <v>86421</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:31">
       <c r="A73" s="1" t="s">
         <v>605</v>
       </c>
@@ -9751,7 +9761,7 @@
         <v>86421</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:31">
       <c r="A74" s="1" t="s">
         <v>606</v>
       </c>
@@ -9846,7 +9856,7 @@
         <v>86710</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:31">
       <c r="A75" s="1" t="s">
         <v>607</v>
       </c>
@@ -9941,7 +9951,7 @@
         <v>86522</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:31">
       <c r="A76" s="1" t="s">
         <v>608</v>
       </c>
@@ -10036,7 +10046,7 @@
         <v>86620</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:31">
       <c r="A77" s="1" t="s">
         <v>609</v>
       </c>
@@ -10129,7 +10139,7 @@
       </c>
       <c r="AE77" s="1"/>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:31">
       <c r="A78" s="1" t="s">
         <v>610</v>
       </c>
@@ -10222,7 +10232,7 @@
       </c>
       <c r="AE78" s="1"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:31">
       <c r="A79" s="1" t="s">
         <v>611</v>
       </c>
@@ -10317,7 +10327,7 @@
         <v>15220</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:31">
       <c r="A80" s="1" t="s">
         <v>612</v>
       </c>
@@ -10412,7 +10422,7 @@
         <v>15430</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:31">
       <c r="A81" s="1" t="s">
         <v>613</v>
       </c>
@@ -10505,7 +10515,7 @@
       </c>
       <c r="AE81" s="1"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:31">
       <c r="A82" s="1" t="s">
         <v>614</v>
       </c>
@@ -10600,7 +10610,7 @@
         <v>15810</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:31">
       <c r="A83" s="1" t="s">
         <v>615</v>
       </c>
@@ -10693,7 +10703,7 @@
       </c>
       <c r="AE83" s="1"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:31">
       <c r="A84" s="1" t="s">
         <v>616</v>
       </c>
@@ -10786,7 +10796,7 @@
       </c>
       <c r="AE84" s="1"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:31">
       <c r="A85" s="1" t="s">
         <v>617</v>
       </c>
@@ -10881,7 +10891,7 @@
         <v>15620</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:31">
       <c r="A86" s="1" t="s">
         <v>246</v>
       </c>
@@ -10976,7 +10986,7 @@
         <v>53221</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:31">
       <c r="A87" s="1" t="s">
         <v>249</v>
       </c>
@@ -11071,7 +11081,7 @@
         <v>53231</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:31">
       <c r="A88" s="1" t="s">
         <v>618</v>
       </c>
@@ -11166,7 +11176,7 @@
         <v>53951</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:31">
       <c r="A89" s="1" t="s">
         <v>619</v>
       </c>
@@ -11261,7 +11271,7 @@
         <v>53220</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:31">
       <c r="A90" s="1" t="s">
         <v>254</v>
       </c>
@@ -11356,7 +11366,7 @@
         <v>53230</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:31">
       <c r="A91" s="1" t="s">
         <v>257</v>
       </c>
@@ -11449,7 +11459,7 @@
       </c>
       <c r="AE91" s="1"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:31">
       <c r="A92" s="1" t="s">
         <v>620</v>
       </c>
@@ -11544,7 +11554,7 @@
         <v>32610</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:31">
       <c r="A93" s="1" t="s">
         <v>621</v>
       </c>
@@ -11639,7 +11649,7 @@
         <v>32630</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:31">
       <c r="A94" s="1" t="s">
         <v>622</v>
       </c>
@@ -11734,7 +11744,7 @@
         <v>32061</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:31">
       <c r="A95" s="1" t="s">
         <v>266</v>
       </c>
@@ -11829,7 +11839,7 @@
         <v>32720</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:31">
       <c r="A96" s="1" t="s">
         <v>269</v>
       </c>
@@ -11914,13 +11924,15 @@
       <c r="AB96" s="1">
         <v>0</v>
       </c>
-      <c r="AC96" s="1"/>
+      <c r="AC96" s="3">
+        <v>8647</v>
+      </c>
       <c r="AD96" s="1">
         <v>436</v>
       </c>
       <c r="AE96" s="1"/>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:31">
       <c r="A97" s="1" t="s">
         <v>272</v>
       </c>
@@ -12013,7 +12025,7 @@
       </c>
       <c r="AE97" s="1"/>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:31">
       <c r="A98" s="1" t="s">
         <v>275</v>
       </c>
@@ -12106,7 +12118,7 @@
       </c>
       <c r="AE98" s="1"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:31">
       <c r="A99" s="1" t="s">
         <v>278</v>
       </c>
@@ -12199,7 +12211,7 @@
       </c>
       <c r="AE99" s="1"/>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:31">
       <c r="A100" s="1" t="s">
         <v>281</v>
       </c>
@@ -12294,7 +12306,7 @@
         <v>32213</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:31">
       <c r="A101" s="1" t="s">
         <v>284</v>
       </c>
@@ -12389,7 +12401,7 @@
         <v>32212</v>
       </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:31">
       <c r="A102" s="1" t="s">
         <v>287</v>
       </c>
@@ -12480,7 +12492,7 @@
       <c r="AD102" s="1"/>
       <c r="AE102" s="1"/>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:31">
       <c r="A103" s="1" t="s">
         <v>290</v>
       </c>
@@ -12575,7 +12587,7 @@
         <v>32230</v>
       </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:31">
       <c r="A104" s="1" t="s">
         <v>293</v>
       </c>
@@ -12670,7 +12682,7 @@
         <v>87423</v>
       </c>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:31">
       <c r="A105" s="1" t="s">
         <v>297</v>
       </c>
@@ -12763,7 +12775,7 @@
       </c>
       <c r="AE105" s="1"/>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:31">
       <c r="A106" s="1" t="s">
         <v>300</v>
       </c>
@@ -12856,7 +12868,7 @@
       </c>
       <c r="AE106" s="1"/>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:31">
       <c r="A107" s="1" t="s">
         <v>303</v>
       </c>
@@ -12951,7 +12963,7 @@
         <v>87310</v>
       </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:31">
       <c r="A108" s="1" t="s">
         <v>306</v>
       </c>
@@ -13046,7 +13058,7 @@
         <v>87320</v>
       </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:31">
       <c r="A109" s="1" t="s">
         <v>309</v>
       </c>
@@ -13141,7 +13153,7 @@
         <v>87620</v>
       </c>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:31">
       <c r="A110" s="1" t="s">
         <v>312</v>
       </c>
@@ -13236,7 +13248,7 @@
         <v>87721</v>
       </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:31">
       <c r="A111" s="1" t="s">
         <v>315</v>
       </c>
@@ -13331,7 +13343,7 @@
         <v>88440</v>
       </c>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:31">
       <c r="A112" s="1" t="s">
         <v>319</v>
       </c>
@@ -13426,7 +13438,7 @@
         <v>88952</v>
       </c>
     </row>
-    <row r="113" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:31">
       <c r="A113" s="1" t="s">
         <v>322</v>
       </c>
@@ -13519,7 +13531,7 @@
       </c>
       <c r="AE113" s="1"/>
     </row>
-    <row r="114" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:31">
       <c r="A114" s="1" t="s">
         <v>324</v>
       </c>
@@ -13614,7 +13626,7 @@
         <v>88710</v>
       </c>
     </row>
-    <row r="115" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:31">
       <c r="A115" s="1" t="s">
         <v>327</v>
       </c>
@@ -13707,7 +13719,7 @@
       </c>
       <c r="AE115" s="1"/>
     </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:31">
       <c r="A116" s="1" t="s">
         <v>330</v>
       </c>
@@ -13800,7 +13812,7 @@
       </c>
       <c r="AE116" s="1"/>
     </row>
-    <row r="117" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:31">
       <c r="A117" s="1" t="s">
         <v>332</v>
       </c>
@@ -13891,7 +13903,7 @@
       </c>
       <c r="AE117" s="1"/>
     </row>
-    <row r="118" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:31">
       <c r="A118" s="1" t="s">
         <v>335</v>
       </c>
@@ -13984,7 +13996,7 @@
       </c>
       <c r="AE118" s="1"/>
     </row>
-    <row r="119" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:31">
       <c r="A119" s="1" t="s">
         <v>338</v>
       </c>
@@ -14077,7 +14089,7 @@
       </c>
       <c r="AE119" s="1"/>
     </row>
-    <row r="120" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:31">
       <c r="A120" s="1" t="s">
         <v>340</v>
       </c>
@@ -14172,7 +14184,7 @@
         <v>88630</v>
       </c>
     </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:31">
       <c r="A121" s="1" t="s">
         <v>623</v>
       </c>
@@ -14267,7 +14279,7 @@
         <v>88460</v>
       </c>
     </row>
-    <row r="122" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:31">
       <c r="A122" s="1" t="s">
         <v>624</v>
       </c>
@@ -14362,7 +14374,7 @@
         <v>23951</v>
       </c>
     </row>
-    <row r="123" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:31">
       <c r="A123" s="1" t="s">
         <v>625</v>
       </c>
@@ -14457,7 +14469,7 @@
         <v>23230</v>
       </c>
     </row>
-    <row r="124" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:31">
       <c r="A124" s="1" t="s">
         <v>626</v>
       </c>
@@ -14552,7 +14564,7 @@
         <v>23220</v>
       </c>
     </row>
-    <row r="125" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:31">
       <c r="A125" s="1" t="s">
         <v>352</v>
       </c>
@@ -14645,7 +14657,7 @@
       </c>
       <c r="AE125" s="1"/>
     </row>
-    <row r="126" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:31">
       <c r="A126" s="1" t="s">
         <v>354</v>
       </c>
@@ -14740,7 +14752,7 @@
         <v>22953</v>
       </c>
     </row>
-    <row r="127" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:31">
       <c r="A127" s="1" t="s">
         <v>356</v>
       </c>
@@ -14835,7 +14847,7 @@
         <v>22711</v>
       </c>
     </row>
-    <row r="128" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:31">
       <c r="A128" s="1" t="s">
         <v>359</v>
       </c>
@@ -14930,7 +14942,7 @@
         <v>22730</v>
       </c>
     </row>
-    <row r="129" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:31">
       <c r="A129" s="1" t="s">
         <v>362</v>
       </c>
@@ -15025,7 +15037,7 @@
         <v>22527</v>
       </c>
     </row>
-    <row r="130" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:31">
       <c r="A130" s="1" t="s">
         <v>365</v>
       </c>
@@ -15120,7 +15132,7 @@
         <v>22430</v>
       </c>
     </row>
-    <row r="131" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:31">
       <c r="A131" s="1" t="s">
         <v>367</v>
       </c>
@@ -15215,7 +15227,7 @@
         <v>22720</v>
       </c>
     </row>
-    <row r="132" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:31">
       <c r="A132" s="1" t="s">
         <v>370</v>
       </c>
@@ -15310,7 +15322,7 @@
         <v>22951</v>
       </c>
     </row>
-    <row r="133" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:31">
       <c r="A133" s="1" t="s">
         <v>373</v>
       </c>
@@ -15405,7 +15417,7 @@
         <v>22722</v>
       </c>
     </row>
-    <row r="134" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:31">
       <c r="A134" s="1" t="s">
         <v>376</v>
       </c>
@@ -15500,7 +15512,7 @@
         <v>22220</v>
       </c>
     </row>
-    <row r="135" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:31">
       <c r="A135" s="1" t="s">
         <v>378</v>
       </c>
@@ -15595,7 +15607,7 @@
         <v>22952</v>
       </c>
     </row>
-    <row r="136" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:31">
       <c r="A136" s="1" t="s">
         <v>381</v>
       </c>
@@ -15690,7 +15702,7 @@
         <v>12951</v>
       </c>
     </row>
-    <row r="137" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:31">
       <c r="A137" s="1" t="s">
         <v>384</v>
       </c>
@@ -15785,7 +15797,7 @@
         <v>12520</v>
       </c>
     </row>
-    <row r="138" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:31">
       <c r="A138" s="1" t="s">
         <v>387</v>
       </c>
@@ -15878,7 +15890,7 @@
       </c>
       <c r="AE138" s="1"/>
     </row>
-    <row r="139" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:31">
       <c r="A139" s="1" t="s">
         <v>627</v>
       </c>
@@ -15971,7 +15983,7 @@
       </c>
       <c r="AE139" s="1"/>
     </row>
-    <row r="140" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:31">
       <c r="A140" s="1" t="s">
         <v>392</v>
       </c>
@@ -16066,7 +16078,7 @@
         <v>12810</v>
       </c>
     </row>
-    <row r="141" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:31">
       <c r="A141" s="1" t="s">
         <v>393</v>
       </c>
@@ -16161,7 +16173,7 @@
         <v>12221</v>
       </c>
     </row>
-    <row r="142" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:31">
       <c r="A142" s="1" t="s">
         <v>628</v>
       </c>
@@ -16254,7 +16266,7 @@
       </c>
       <c r="AE142" s="1"/>
     </row>
-    <row r="143" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:31">
       <c r="A143" s="1" t="s">
         <v>399</v>
       </c>
@@ -16347,7 +16359,7 @@
       </c>
       <c r="AE143" s="1"/>
     </row>
-    <row r="144" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:31">
       <c r="A144" s="1" t="s">
         <v>401</v>
       </c>
@@ -16440,7 +16452,7 @@
       </c>
       <c r="AE144" s="1"/>
     </row>
-    <row r="145" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:31">
       <c r="A145" s="1" t="s">
         <v>403</v>
       </c>
@@ -16531,7 +16543,7 @@
       </c>
       <c r="AE145" s="1"/>
     </row>
-    <row r="146" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:31">
       <c r="A146" s="1" t="s">
         <v>406</v>
       </c>
@@ -16626,7 +16638,7 @@
         <v>92713</v>
       </c>
     </row>
-    <row r="147" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:31">
       <c r="A147" s="1" t="s">
         <v>409</v>
       </c>
@@ -16719,7 +16731,7 @@
       </c>
       <c r="AE147" s="1"/>
     </row>
-    <row r="148" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:31">
       <c r="A148" s="1" t="s">
         <v>412</v>
       </c>
@@ -16814,7 +16826,7 @@
         <v>92712</v>
       </c>
     </row>
-    <row r="149" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:31">
       <c r="A149" s="1" t="s">
         <v>415</v>
       </c>
@@ -16907,7 +16919,7 @@
       </c>
       <c r="AE149" s="1"/>
     </row>
-    <row r="150" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:31">
       <c r="A150" s="1" t="s">
         <v>418</v>
       </c>
@@ -16998,7 +17010,7 @@
       </c>
       <c r="AE150" s="1"/>
     </row>
-    <row r="151" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:31">
       <c r="A151" s="1" t="s">
         <v>421</v>
       </c>
@@ -17093,7 +17105,7 @@
         <v>92436</v>
       </c>
     </row>
-    <row r="152" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:31">
       <c r="A152" s="1" t="s">
         <v>424</v>
       </c>
@@ -17186,7 +17198,7 @@
       </c>
       <c r="AE152" s="1"/>
     </row>
-    <row r="153" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:31">
       <c r="A153" s="1" t="s">
         <v>426</v>
       </c>
@@ -17281,7 +17293,7 @@
         <v>92621</v>
       </c>
     </row>
-    <row r="154" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:31">
       <c r="A154" s="1" t="s">
         <v>429</v>
       </c>
@@ -17376,7 +17388,7 @@
         <v>92622</v>
       </c>
     </row>
-    <row r="155" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:31">
       <c r="A155" s="1" t="s">
         <v>432</v>
       </c>
@@ -17471,7 +17483,7 @@
         <v>92432</v>
       </c>
     </row>
-    <row r="156" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:31">
       <c r="A156" s="1" t="s">
         <v>435</v>
       </c>
@@ -17564,7 +17576,7 @@
       </c>
       <c r="AE156" s="1"/>
     </row>
-    <row r="157" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:31">
       <c r="A157" s="1" t="s">
         <v>438</v>
       </c>
@@ -17659,7 +17671,7 @@
         <v>35211</v>
       </c>
     </row>
-    <row r="158" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:31">
       <c r="A158" s="1" t="s">
         <v>442</v>
       </c>
@@ -17750,7 +17762,7 @@
       </c>
       <c r="AE158" s="1"/>
     </row>
-    <row r="159" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:31">
       <c r="A159" s="1" t="s">
         <v>629</v>
       </c>
@@ -17845,7 +17857,7 @@
         <v>35229</v>
       </c>
     </row>
-    <row r="160" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:31">
       <c r="A160" s="1" t="s">
         <v>630</v>
       </c>
@@ -17940,7 +17952,7 @@
         <v>35220</v>
       </c>
     </row>
-    <row r="161" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31">
       <c r="A161" s="1" t="s">
         <v>631</v>
       </c>
@@ -18035,7 +18047,7 @@
         <v>93981</v>
       </c>
     </row>
-    <row r="162" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31">
       <c r="A162" s="1" t="s">
         <v>632</v>
       </c>
@@ -18130,7 +18142,7 @@
         <v>93712</v>
       </c>
     </row>
-    <row r="163" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31">
       <c r="A163" s="1" t="s">
         <v>633</v>
       </c>
@@ -18223,7 +18235,7 @@
       </c>
       <c r="AE163" s="1"/>
     </row>
-    <row r="164" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31">
       <c r="A164" s="1" t="s">
         <v>456</v>
       </c>
@@ -18318,7 +18330,7 @@
         <v>93713</v>
       </c>
     </row>
-    <row r="165" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31">
       <c r="A165" s="1" t="s">
         <v>634</v>
       </c>
@@ -18413,7 +18425,7 @@
         <v>93222</v>
       </c>
     </row>
-    <row r="166" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31">
       <c r="A166" s="1" t="s">
         <v>461</v>
       </c>
@@ -18508,7 +18520,7 @@
         <v>93711</v>
       </c>
     </row>
-    <row r="167" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31">
       <c r="A167" s="1" t="s">
         <v>635</v>
       </c>
@@ -18603,7 +18615,7 @@
         <v>96424</v>
       </c>
     </row>
-    <row r="168" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31">
       <c r="A168" s="1" t="s">
         <v>636</v>
       </c>
@@ -18698,7 +18710,7 @@
         <v>96222</v>
       </c>
     </row>
-    <row r="169" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31">
       <c r="A169" s="1" t="s">
         <v>637</v>
       </c>
@@ -18793,7 +18805,7 @@
         <v>96720</v>
       </c>
     </row>
-    <row r="170" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31">
       <c r="A170" s="1" t="s">
         <v>638</v>
       </c>
@@ -18888,7 +18900,7 @@
         <v>96610</v>
       </c>
     </row>
-    <row r="171" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31">
       <c r="A171" s="1" t="s">
         <v>639</v>
       </c>
@@ -18983,7 +18995,7 @@
         <v>96620</v>
       </c>
     </row>
-    <row r="172" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31">
       <c r="A172" s="1" t="s">
         <v>640</v>
       </c>
@@ -19076,7 +19088,7 @@
       </c>
       <c r="AE172" s="1"/>
     </row>
-    <row r="173" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31">
       <c r="A173" s="1" t="s">
         <v>476</v>
       </c>
@@ -19171,7 +19183,7 @@
         <v>96440</v>
       </c>
     </row>
-    <row r="174" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31">
       <c r="A174" s="1" t="s">
         <v>641</v>
       </c>
@@ -19266,7 +19278,7 @@
         <v>96710</v>
       </c>
     </row>
-    <row r="175" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31">
       <c r="A175" s="1" t="s">
         <v>642</v>
       </c>
@@ -19361,7 +19373,7 @@
         <v>96725</v>
       </c>
     </row>
-    <row r="176" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31">
       <c r="A176" s="1" t="s">
         <v>643</v>
       </c>
@@ -19456,7 +19468,7 @@
         <v>96423</v>
       </c>
     </row>
-    <row r="177" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:31">
       <c r="A177" s="1" t="s">
         <v>644</v>
       </c>
@@ -19551,7 +19563,7 @@
         <v>96422</v>
       </c>
     </row>
-    <row r="178" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:31">
       <c r="A178" s="1" t="s">
         <v>645</v>
       </c>
@@ -19646,7 +19658,7 @@
         <v>96210</v>
       </c>
     </row>
-    <row r="179" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:31">
       <c r="A179" s="1" t="s">
         <v>489</v>
       </c>
@@ -19739,7 +19751,7 @@
       </c>
       <c r="AE179" s="1"/>
     </row>
-    <row r="180" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:31">
       <c r="A180" s="1" t="s">
         <v>646</v>
       </c>
@@ -19832,7 +19844,7 @@
       </c>
       <c r="AE180" s="1"/>
     </row>
-    <row r="181" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:31">
       <c r="A181" s="1" t="s">
         <v>495</v>
       </c>
@@ -19927,7 +19939,7 @@
         <v>97330</v>
       </c>
     </row>
-    <row r="182" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:31">
       <c r="A182" s="1" t="s">
         <v>498</v>
       </c>
@@ -20022,7 +20034,7 @@
         <v>97710</v>
       </c>
     </row>
-    <row r="183" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:31">
       <c r="A183" s="1" t="s">
         <v>500</v>
       </c>
@@ -20115,7 +20127,7 @@
       </c>
       <c r="AE183" s="1"/>
     </row>
-    <row r="184" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:31">
       <c r="A184" s="1" t="s">
         <v>647</v>
       </c>
@@ -20210,7 +20222,7 @@
         <v>97321</v>
       </c>
     </row>
-    <row r="185" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:31">
       <c r="A185" s="1" t="s">
         <v>505</v>
       </c>
@@ -20305,7 +20317,7 @@
         <v>33908</v>
       </c>
     </row>
-    <row r="186" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:31">
       <c r="A186" s="1" t="s">
         <v>509</v>
       </c>
@@ -20390,13 +20402,15 @@
       <c r="AB186" s="1">
         <v>0</v>
       </c>
-      <c r="AC186" s="1"/>
+      <c r="AC186" s="3">
+        <v>1564</v>
+      </c>
       <c r="AD186" s="1">
         <v>1367</v>
       </c>
       <c r="AE186" s="1"/>
     </row>
-    <row r="187" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:31">
       <c r="A187" s="1" t="s">
         <v>648</v>
       </c>
@@ -20491,7 +20505,7 @@
         <v>33098</v>
       </c>
     </row>
-    <row r="188" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:31">
       <c r="A188" s="1" t="s">
         <v>649</v>
       </c>
@@ -20586,7 +20600,7 @@
         <v>33096</v>
       </c>
     </row>
-    <row r="189" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:31">
       <c r="A189" s="1" t="s">
         <v>516</v>
       </c>
@@ -20681,7 +20695,7 @@
         <v>33097</v>
       </c>
     </row>
-    <row r="190" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:31">
       <c r="A190" s="1" t="s">
         <v>519</v>
       </c>
@@ -20776,7 +20790,7 @@
         <v>33095</v>
       </c>
     </row>
-    <row r="191" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:31">
       <c r="A191" s="1" t="s">
         <v>650</v>
       </c>
@@ -20867,7 +20881,7 @@
       </c>
       <c r="AE191" s="1"/>
     </row>
-    <row r="192" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:31">
       <c r="A192" s="1" t="s">
         <v>524</v>
       </c>
@@ -20960,7 +20974,7 @@
       </c>
       <c r="AE192" s="1"/>
     </row>
-    <row r="193" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:31">
       <c r="A193" s="1" t="s">
         <v>527</v>
       </c>
@@ -21055,7 +21069,7 @@
         <v>33220</v>
       </c>
     </row>
-    <row r="194" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:31">
       <c r="A194" s="1" t="s">
         <v>530</v>
       </c>
@@ -21150,7 +21164,7 @@
         <v>33210</v>
       </c>
     </row>
-    <row r="195" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:31">
       <c r="A195" s="1" t="s">
         <v>531</v>
       </c>
@@ -21243,7 +21257,7 @@
       </c>
       <c r="AE195" s="1"/>
     </row>
-    <row r="196" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:31">
       <c r="A196" s="1" t="s">
         <v>533</v>
       </c>
@@ -21338,7 +21352,7 @@
         <v>11951</v>
       </c>
     </row>
-    <row r="197" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:31">
       <c r="A197" s="1" t="s">
         <v>537</v>
       </c>
@@ -21433,7 +21447,7 @@
         <v>11710</v>
       </c>
     </row>
-    <row r="198" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:31">
       <c r="A198" s="1" t="s">
         <v>651</v>
       </c>
@@ -21528,7 +21542,7 @@
         <v>11220</v>
       </c>
     </row>
-    <row r="199" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:31">
       <c r="A199" s="1" t="s">
         <v>542</v>
       </c>
@@ -21623,7 +21637,7 @@
         <v>43951</v>
       </c>
     </row>
-    <row r="200" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:31">
       <c r="A200" s="1" t="s">
         <v>652</v>
       </c>
@@ -21718,7 +21732,7 @@
         <v>43711</v>
       </c>
     </row>
-    <row r="201" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:31">
       <c r="A201" s="1" t="s">
         <v>548</v>
       </c>
@@ -21813,7 +21827,7 @@
         <v>43901</v>
       </c>
     </row>
-    <row r="202" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:31">
       <c r="A202" s="1" t="s">
         <v>551</v>
       </c>
@@ -21904,7 +21918,7 @@
       </c>
       <c r="AE202" s="1"/>
     </row>
-    <row r="203" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:31">
       <c r="A203" s="1" t="s">
         <v>653</v>
       </c>
@@ -21999,7 +22013,7 @@
         <v>43710</v>
       </c>
     </row>
-    <row r="204" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:31">
       <c r="A204" s="1" t="s">
         <v>556</v>
       </c>
@@ -22094,7 +22108,7 @@
         <v>43220</v>
       </c>
     </row>
-    <row r="205" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:31">
       <c r="A205" s="1" t="s">
         <v>559</v>
       </c>
@@ -22187,7 +22201,7 @@
       </c>
       <c r="AE205" s="1"/>
     </row>
-    <row r="206" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:31">
       <c r="A206" s="1" t="s">
         <v>654</v>
       </c>
@@ -22282,7 +22296,7 @@
         <v>43810</v>
       </c>
     </row>
-    <row r="207" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:31">
       <c r="A207" s="1" t="s">
         <v>655</v>
       </c>
@@ -22377,7 +22391,7 @@
         <v>43902</v>
       </c>
     </row>
-    <row r="208" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:31">
       <c r="A208" s="1" t="s">
         <v>566</v>
       </c>
@@ -22472,7 +22486,7 @@
         <v>51620</v>
       </c>
     </row>
-    <row r="209" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:31">
       <c r="A209" s="1" t="s">
         <v>569</v>
       </c>
@@ -22567,7 +22581,7 @@
         <v>51903</v>
       </c>
     </row>
-    <row r="210" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:31">
       <c r="A210" s="1" t="s">
         <v>656</v>
       </c>
@@ -22658,7 +22672,7 @@
       </c>
       <c r="AE210" s="1"/>
     </row>
-    <row r="211" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:31">
       <c r="A211" s="1" t="s">
         <v>618</v>
       </c>
@@ -22753,7 +22767,7 @@
         <v>51210</v>
       </c>
     </row>
-    <row r="212" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:31">
       <c r="A212" s="1" t="s">
         <v>574</v>
       </c>
@@ -22850,5 +22864,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>